<commit_message>
GameManager를 PeekabooGameManager와 구분하기, TestDB 삭제
</commit_message>
<xml_diff>
--- a/KGA_SUPERmetaVR/Assets/Sheet/Data.xlsx
+++ b/KGA_SUPERmetaVR/Assets/Sheet/Data.xlsx
@@ -4,37 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="TestDB" sheetId="1" r:id="rId1"/>
-    <sheet name="NoticePopup" sheetId="3" r:id="rId2"/>
-    <sheet name="PeekabooCustomizing" sheetId="4" r:id="rId3"/>
+    <sheet name="NoticePopup" sheetId="3" r:id="rId1"/>
+    <sheet name="PeekabooCustomizing" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>one</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>two</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>text</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -167,11 +150,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -488,48 +468,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="18.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.75" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>100</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>101</v>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -541,89 +548,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F7:F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="18.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.75" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -635,87 +562,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>301</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>302</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5">
-        <v>301</v>
-      </c>
-      <c r="C2" s="5" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>303</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5">
-        <v>302</v>
-      </c>
-      <c r="C3" s="5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>304</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5">
-        <v>303</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>305</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5">
-        <v>304</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5">
-        <v>305</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
StaticData에 Item 추가, ItemSheet로 이름 변경
</commit_message>
<xml_diff>
--- a/KGA_SUPERmetaVR/Assets/Sheet/Data.xlsx
+++ b/KGA_SUPERmetaVR/Assets/Sheet/Data.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NoticePopup" sheetId="3" r:id="rId1"/>
     <sheet name="PeekabooCustomizing" sheetId="4" r:id="rId2"/>
     <sheet name="SpeechBubbleSheet" sheetId="5" r:id="rId3"/>
+    <sheet name="ItemSheet" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -126,6 +127,43 @@
   </si>
   <si>
     <t>SpeechText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discription</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PrefabName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 아이템은 테스트를 위하여 추가된 아이템1입니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 아이템은 테스트를 위하여 추가된 아이템2입니다.
+두 줄 테스트 및 아이템 비교를 위하여 추가되었습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -686,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -742,4 +780,70 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="16.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="22.125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>60001</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>60002</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'main' into InventoryUI_RWJ"
This reverts commit b4326dd03305f33487d36acb853ae46e0ffcee42, reversing
changes made to 9592bf2a2aae77ad3c816e3b3e9d41f8b977b6a1.
</commit_message>
<xml_diff>
--- a/KGA_SUPERmetaVR/Assets/Sheet/Data.xlsx
+++ b/KGA_SUPERmetaVR/Assets/Sheet/Data.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Slime\VR\SUPERmeta\KGA_SUPERmetaVR\Assets\Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohgo\Desktop\Unity\SUPERmetaVR\KGA_SUPERmetaVR\KGA_SUPERmetaVR\Assets\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA00017-3EEA-4F4C-89EB-4FFE03E432B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NoticePopup" sheetId="1" r:id="rId1"/>
-    <sheet name="NPCSheet" sheetId="7" r:id="rId2"/>
-    <sheet name="NPCDialogue" sheetId="5" r:id="rId3"/>
-    <sheet name="PeekabooCustomizing" sheetId="2" r:id="rId4"/>
-    <sheet name="SpeechBubbleSheet" sheetId="3" r:id="rId5"/>
-    <sheet name="ItemSheet" sheetId="4" r:id="rId6"/>
-    <sheet name="RewardSheet" sheetId="6" r:id="rId7"/>
+    <sheet name="NPCDialogue" sheetId="5" r:id="rId2"/>
+    <sheet name="PeekabooCustomizing" sheetId="2" r:id="rId3"/>
+    <sheet name="SpeechBubbleSheet" sheetId="3" r:id="rId4"/>
+    <sheet name="ItemSheet" sheetId="4" r:id="rId5"/>
+    <sheet name="RewardSheet" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="185">
   <si>
     <t>id</t>
   </si>
@@ -585,6 +585,9 @@
 네 잎 클로버를 4개 모으면 말해!</t>
   </si>
   <si>
+    <t>코스튬이 갖고 싶으면 네 잎 클로버 4개를 가져와!</t>
+  </si>
+  <si>
     <t>안녕, 친구.
 재미있는 놀이가 하나 있는데 이야기해줄까?</t>
   </si>
@@ -813,6 +816,564 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>개를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>모았으면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>언제든지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>말을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>걸어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>!</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>안녕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>나는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>코티야</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>네</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>잎</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>클로버를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>가져오면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>코스튬으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>변화시켜줄게</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>됐어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>이쁘게</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>착용해</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-!</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>좋아</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ~
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>우리</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>미니마니모</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>마을엔</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>인간과</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>사이좋게</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>지내고싶은</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>도깨비들이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>많아</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>네잎클로버</t>
   </si>
   <si>
@@ -984,167 +1545,13 @@
   </si>
   <si>
     <t>Sword</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SoudEffect</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetItemID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetItemEA</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>OutItemID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>OutItemEA</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Animation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>TT_Mo_1.wav</t>
-  </si>
-  <si>
-    <t>TT_Mo_2.wav</t>
-  </si>
-  <si>
-    <t>TT_Mo_3.wav</t>
-  </si>
-  <si>
-    <t>TT_Cu_1.wav</t>
-  </si>
-  <si>
-    <t>TT_Cu_3.mp3</t>
-  </si>
-  <si>
-    <t>TT_Cu_2.mp3</t>
-  </si>
-  <si>
-    <t>안녕? 적응은 잘 하고있어? 즐거운 하루 보내!</t>
-  </si>
-  <si>
-    <t>나는 여기서 항상 새로운 어린이들을 인도해!</t>
-  </si>
-  <si>
-    <t>쿠가 좀 까칠하지? 하지만 마음은 따듯한 녀석이야-</t>
-  </si>
-  <si>
-    <t>이 쿠님이 보고싶어서 왔나?</t>
-  </si>
-  <si>
-    <t>어린이- 저기가서 놀아- 이 쿠님은 바쁘다고-</t>
-  </si>
-  <si>
-    <t>안녕- 나는 코티야. 네 잎 클로버를 4개 가져오면 코스튬으로 변화시켜줄게</t>
-  </si>
-  <si>
-    <t>CC_Coty_1.mp3</t>
-  </si>
-  <si>
-    <t>4개를 모았으면 언제든지 말을 걸어!</t>
-  </si>
-  <si>
-    <t>CC_Coty_2.mp3</t>
-  </si>
-  <si>
-    <t>CC_Coty_3.mp3</t>
-  </si>
-  <si>
-    <t>다 됐어-! 이쁘게 착용해-!</t>
-  </si>
-  <si>
-    <t>CC_Coty_4.mp3</t>
-  </si>
-  <si>
-    <t>음? 코스튬이 갖고 싶으면 네 잎 클로버 4개를 가져와!</t>
-  </si>
-  <si>
-    <t>CC_Coty_5.mp3</t>
-  </si>
-  <si>
-    <t>PK_BOO_1.mp3</t>
-  </si>
-  <si>
-    <t>좋아 ~
-우리 미니마니모 마을엔 인간과 사이좋게 지내고싶은 도깨비들이 많아</t>
-  </si>
-  <si>
-    <t>PK_BOO_2.mp3</t>
-  </si>
-  <si>
-    <t>모</t>
-  </si>
-  <si>
-    <t>쿠</t>
-  </si>
-  <si>
-    <t>코티</t>
-  </si>
-  <si>
-    <t>부</t>
-  </si>
-  <si>
-    <r>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ame</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ype</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nimation</t>
-    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
@@ -1514,23 +1921,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" style="9" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" style="9" customWidth="1"/>
     <col min="3" max="3" width="92" style="9" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" style="9" customWidth="1"/>
     <col min="6" max="7" width="9" style="9" customWidth="1"/>
-    <col min="8" max="27" width="8.7109375" style="9" customWidth="1"/>
-    <col min="28" max="16384" width="14.42578125" style="9"/>
+    <col min="8" max="27" width="8.7265625" style="9" customWidth="1"/>
+    <col min="28" max="16384" width="14.453125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.5" customHeight="1">
@@ -1572,7 +1979,7 @@
       <c r="Z1" s="6"/>
       <c r="AA1" s="6"/>
     </row>
-    <row r="2" spans="1:27" ht="30">
+    <row r="2" spans="1:27" ht="29">
       <c r="A2" s="11">
         <v>0</v>
       </c>
@@ -1837,7 +2244,7 @@
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
     </row>
-    <row r="9" spans="1:27" ht="30">
+    <row r="9" spans="1:27" ht="29">
       <c r="A9" s="11">
         <v>52004</v>
       </c>
@@ -2022,7 +2429,7 @@
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
     </row>
-    <row r="14" spans="1:27" ht="30">
+    <row r="14" spans="1:27" ht="29">
       <c r="A14" s="11">
         <v>52009</v>
       </c>
@@ -2082,168 +2489,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="9"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="1" max="3" width="9.1796875" style="15"/>
+    <col min="4" max="4" width="82.54296875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="15" customWidth="1"/>
+    <col min="6" max="9" width="29.26953125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" style="15" customWidth="1"/>
+    <col min="11" max="14" width="29.26953125" style="15" customWidth="1"/>
+    <col min="15" max="16384" width="9.1796875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1">
-      <c r="A1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="9">
-        <v>20000</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="9">
-        <v>20001</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="9">
-        <v>20300</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="9">
-        <v>20600</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="9.140625" style="15"/>
-    <col min="4" max="4" width="82.5703125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="15" customWidth="1"/>
-    <col min="6" max="9" width="29.28515625" style="15" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="15" customWidth="1"/>
-    <col min="11" max="14" width="29.28515625" style="15" customWidth="1"/>
-    <col min="15" max="20" width="14.85546875" style="16" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" s="15" customFormat="1">
+    <row r="1" spans="1:14" s="15" customFormat="1">
       <c r="A1" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>120</v>
-      </c>
       <c r="I1" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="R1" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="S1" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="T1" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="15">
-        <v>21000</v>
+        <v>21001</v>
       </c>
       <c r="B2" s="15">
         <v>20000</v>
@@ -2252,10 +2562,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="30">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="29">
       <c r="A3" s="15">
         <v>21001</v>
       </c>
@@ -2263,16 +2573,13 @@
         <v>20000</v>
       </c>
       <c r="C3" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="O3" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="30">
+    </row>
+    <row r="4" spans="1:14" ht="29">
       <c r="A4" s="15">
         <v>21001</v>
       </c>
@@ -2280,16 +2587,13 @@
         <v>20000</v>
       </c>
       <c r="C4" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="O4" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="30">
+    </row>
+    <row r="5" spans="1:14" ht="29">
       <c r="A5" s="15">
         <v>21001</v>
       </c>
@@ -2297,13 +2601,13 @@
         <v>20000</v>
       </c>
       <c r="C5" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="30">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="29">
       <c r="A6" s="15">
         <v>21001</v>
       </c>
@@ -2311,13 +2615,13 @@
         <v>20000</v>
       </c>
       <c r="C6" s="15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:14">
       <c r="A7" s="15">
         <v>21001</v>
       </c>
@@ -2325,13 +2629,13 @@
         <v>20000</v>
       </c>
       <c r="C7" s="15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="30">
+    <row r="8" spans="1:14" ht="29">
       <c r="A8" s="15">
         <v>21001</v>
       </c>
@@ -2339,16 +2643,13 @@
         <v>20000</v>
       </c>
       <c r="C8" s="15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" s="20" customFormat="1" ht="30">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="20" customFormat="1" ht="29">
       <c r="A9" s="18">
         <v>21002</v>
       </c>
@@ -2372,7 +2673,7 @@
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
     </row>
-    <row r="10" spans="1:20" ht="30">
+    <row r="10" spans="1:14" ht="29">
       <c r="A10" s="15">
         <v>21003</v>
       </c>
@@ -2383,13 +2684,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="15">
         <v>21003</v>
       </c>
@@ -2403,7 +2701,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="20" customFormat="1">
+    <row r="12" spans="1:14" s="20" customFormat="1">
       <c r="A12" s="18">
         <v>21004</v>
       </c>
@@ -2414,7 +2712,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -2426,11 +2724,8 @@
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
-      <c r="O12" s="20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" s="20" customFormat="1" ht="30">
+    </row>
+    <row r="13" spans="1:14" s="20" customFormat="1" ht="29">
       <c r="A13" s="18">
         <v>21004</v>
       </c>
@@ -2441,7 +2736,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
@@ -2454,7 +2749,7 @@
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="1:20" ht="30">
+    <row r="14" spans="1:14" ht="29">
       <c r="A14" s="15">
         <v>21005</v>
       </c>
@@ -2468,7 +2763,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="30">
+    <row r="15" spans="1:14" ht="29">
       <c r="A15" s="15">
         <v>21005</v>
       </c>
@@ -2482,7 +2777,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="30">
+    <row r="16" spans="1:14" ht="29">
       <c r="A16" s="15">
         <v>21005</v>
       </c>
@@ -2496,7 +2791,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="30">
+    <row r="17" spans="1:14" ht="29">
       <c r="A17" s="15">
         <v>21005</v>
       </c>
@@ -2507,13 +2802,10 @@
         <v>4</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="O17" s="16" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="30">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="29">
       <c r="A18" s="15">
         <v>21005</v>
       </c>
@@ -2524,10 +2816,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="15">
         <v>21005</v>
       </c>
@@ -2538,21 +2830,21 @@
         <v>6</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" s="20" customFormat="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="20" customFormat="1">
       <c r="A20" s="18">
-        <v>21006</v>
+        <v>24000</v>
       </c>
       <c r="B20" s="18">
-        <v>20000</v>
+        <v>20300</v>
       </c>
       <c r="C20" s="18">
         <v>1</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>192</v>
+        <v>131</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
@@ -2564,22 +2856,19 @@
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" s="20" customFormat="1">
+    </row>
+    <row r="21" spans="1:14" s="20" customFormat="1">
       <c r="A21" s="18">
-        <v>21007</v>
+        <v>24000</v>
       </c>
       <c r="B21" s="18">
-        <v>20000</v>
+        <v>20300</v>
       </c>
       <c r="C21" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>193</v>
+        <v>130</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
@@ -2591,39 +2880,48 @@
       <c r="L21" s="18"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19">
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="15">
-        <v>21008</v>
+        <v>24001</v>
       </c>
       <c r="B22" s="15">
-        <v>20000</v>
+        <v>20300</v>
       </c>
       <c r="C22" s="15">
         <v>1</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="O22" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" s="20" customFormat="1">
+        <v>81</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="15">
+        <v>24002</v>
+      </c>
+      <c r="I22" s="15">
+        <v>24003</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="N22" s="15">
+        <v>24004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="20" customFormat="1">
       <c r="A23" s="18">
-        <v>21009</v>
+        <v>24002</v>
       </c>
       <c r="B23" s="18">
-        <v>20001</v>
+        <v>20300</v>
       </c>
       <c r="C23" s="18">
         <v>1</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>195</v>
+        <v>84</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
@@ -2636,18 +2934,18 @@
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="1:19" s="20" customFormat="1">
+    <row r="24" spans="1:14" s="20" customFormat="1">
       <c r="A24" s="18">
-        <v>21010</v>
+        <v>24002</v>
       </c>
       <c r="B24" s="18">
-        <v>20001</v>
+        <v>20300</v>
       </c>
       <c r="C24" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>196</v>
+        <v>132</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
@@ -2660,9 +2958,9 @@
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:14" ht="29">
       <c r="A25" s="15">
-        <v>24000</v>
+        <v>24003</v>
       </c>
       <c r="B25" s="15">
         <v>20300</v>
@@ -2671,24 +2969,21 @@
         <v>1</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="O25" s="16" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" s="20" customFormat="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="20" customFormat="1">
       <c r="A26" s="18">
-        <v>24000</v>
+        <v>24004</v>
       </c>
       <c r="B26" s="18">
         <v>20300</v>
       </c>
       <c r="C26" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>199</v>
+        <v>86</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
@@ -2701,56 +2996,44 @@
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:14" ht="29">
       <c r="A27" s="15">
-        <v>24001</v>
+        <v>27000</v>
       </c>
       <c r="B27" s="15">
-        <v>20300</v>
+        <v>20600</v>
       </c>
       <c r="C27" s="15">
         <v>1</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" s="15">
-        <v>12000</v>
-      </c>
-      <c r="G27" s="15">
-        <v>4</v>
-      </c>
-      <c r="H27" s="15">
-        <v>24002</v>
+        <v>88</v>
       </c>
       <c r="I27" s="15">
-        <v>24003</v>
+        <v>27002</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="N27" s="15">
-        <v>24004</v>
-      </c>
-      <c r="O27" s="16" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" s="20" customFormat="1">
+        <v>27001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="20" customFormat="1" ht="29">
       <c r="A28" s="18">
-        <v>24002</v>
+        <v>27001</v>
       </c>
       <c r="B28" s="18">
-        <v>20300</v>
+        <v>20600</v>
       </c>
       <c r="C28" s="18">
         <v>1</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
@@ -2762,116 +3045,92 @@
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
-      <c r="O28" s="20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19">
+    </row>
+    <row r="29" spans="1:14" ht="29">
       <c r="A29" s="15">
-        <v>24002</v>
+        <v>27002</v>
       </c>
       <c r="B29" s="15">
-        <v>20300</v>
+        <v>20600</v>
       </c>
       <c r="C29" s="15">
+        <v>1</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="29">
+      <c r="A30" s="15">
+        <v>27002</v>
+      </c>
+      <c r="B30" s="15">
+        <v>20600</v>
+      </c>
+      <c r="C30" s="15">
         <v>2</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="P29" s="16">
-        <v>13000</v>
-      </c>
-      <c r="Q29" s="16">
-        <v>1</v>
-      </c>
-      <c r="R29" s="16">
-        <v>12000</v>
-      </c>
-      <c r="S29" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="30">
-      <c r="A30" s="15">
-        <v>24003</v>
-      </c>
-      <c r="B30" s="15">
-        <v>20300</v>
-      </c>
-      <c r="C30" s="15">
-        <v>1</v>
-      </c>
       <c r="D30" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="O30" s="16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="29">
       <c r="A31" s="15">
-        <v>24004</v>
+        <v>27002</v>
       </c>
       <c r="B31" s="15">
-        <v>20300</v>
+        <v>20600</v>
       </c>
       <c r="C31" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="O31" s="16" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="30">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="15">
-        <v>27000</v>
+        <v>27002</v>
       </c>
       <c r="B32" s="15">
         <v>20600</v>
       </c>
       <c r="C32" s="15">
-        <v>1</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="I32" s="15">
+        <v>4</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="29">
+      <c r="A33" s="15">
         <v>27002</v>
-      </c>
-      <c r="J32" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="N32" s="15">
-        <v>27001</v>
-      </c>
-      <c r="O32" s="16" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="30">
-      <c r="A33" s="15">
-        <v>27001</v>
       </c>
       <c r="B33" s="15">
         <v>20600</v>
       </c>
       <c r="C33" s="15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="20" customFormat="1" ht="30">
+        <v>94</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I33" s="15">
+        <v>27006</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="N33" s="15">
+        <v>27003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="20" customFormat="1" ht="29">
       <c r="A34" s="18">
-        <v>27002</v>
+        <v>27003</v>
       </c>
       <c r="B34" s="18">
         <v>20600</v>
@@ -2880,231 +3139,136 @@
         <v>1</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="E34" s="18"/>
+        <v>97</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
+      <c r="I34" s="18">
+        <v>27004</v>
+      </c>
+      <c r="J34" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-    </row>
-    <row r="35" spans="1:15" ht="30">
+      <c r="N34" s="18">
+        <v>27001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="29">
       <c r="A35" s="15">
-        <v>27002</v>
+        <v>27004</v>
       </c>
       <c r="B35" s="15">
         <v>20600</v>
       </c>
       <c r="C35" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="20" customFormat="1" ht="30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="20" customFormat="1">
       <c r="A36" s="18">
-        <v>27002</v>
+        <v>27005</v>
       </c>
       <c r="B36" s="18">
         <v>20600</v>
       </c>
       <c r="C36" s="18">
-        <v>3</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
+      <c r="I36" s="18">
+        <v>27004</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="K36" s="18"/>
       <c r="L36" s="18"/>
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:14">
       <c r="A37" s="15">
-        <v>27002</v>
+        <v>27006</v>
       </c>
       <c r="B37" s="15">
         <v>20600</v>
       </c>
       <c r="C37" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="O37" s="16" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="30">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="29">
       <c r="A38" s="15">
-        <v>27002</v>
+        <v>27006</v>
       </c>
       <c r="B38" s="15">
         <v>20600</v>
       </c>
       <c r="C38" s="15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I38" s="15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="15">
         <v>27006</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="N38" s="15">
-        <v>27003</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="30">
-      <c r="A39" s="15">
-        <v>27003</v>
       </c>
       <c r="B39" s="15">
         <v>20600</v>
       </c>
       <c r="C39" s="15">
-        <v>1</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="I39" s="15">
-        <v>27004</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="N39" s="15">
-        <v>27001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="30">
+        <v>3</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="15">
-        <v>27004</v>
+        <v>27006</v>
       </c>
       <c r="B40" s="15">
         <v>20600</v>
       </c>
       <c r="C40" s="15">
-        <v>1</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15">
-      <c r="A41" s="15">
-        <v>27005</v>
-      </c>
-      <c r="B41" s="15">
-        <v>20600</v>
-      </c>
-      <c r="C41" s="15">
-        <v>1</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="I41" s="15">
-        <v>27004</v>
-      </c>
-      <c r="J41" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="O41" s="16" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15">
-      <c r="A42" s="15">
-        <v>27006</v>
-      </c>
-      <c r="B42" s="15">
-        <v>20600</v>
-      </c>
-      <c r="C42" s="15">
-        <v>1</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="30">
-      <c r="A43" s="15">
-        <v>27006</v>
-      </c>
-      <c r="B43" s="15">
-        <v>20600</v>
-      </c>
-      <c r="C43" s="15">
-        <v>2</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="A44" s="15">
-        <v>27006</v>
-      </c>
-      <c r="B44" s="15">
-        <v>20600</v>
-      </c>
-      <c r="C44" s="15">
-        <v>3</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="A45" s="15">
-        <v>27006</v>
-      </c>
-      <c r="B45" s="15">
-        <v>20600</v>
-      </c>
-      <c r="C45" s="15">
         <v>4</v>
       </c>
-      <c r="D45" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E45" s="15" t="s">
+      <c r="D40" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="I45" s="15">
+      <c r="E40" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="I40" s="15">
         <v>27003</v>
       </c>
-      <c r="J45" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="N45" s="15">
+      <c r="J40" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="N40" s="15">
         <v>27006</v>
       </c>
     </row>
@@ -3115,20 +3279,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
-    <col min="5" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="2" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="4" width="28.26953125" customWidth="1"/>
+    <col min="5" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" customHeight="1">
@@ -3222,20 +3386,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="66.85546875" customWidth="1"/>
+    <col min="2" max="2" width="66.81640625" customWidth="1"/>
     <col min="3" max="6" width="9" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="7" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1">
@@ -3405,23 +3569,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="78.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
     <col min="5" max="5" width="13" style="9" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="7" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="9" customFormat="1" ht="16.5" customHeight="1">
@@ -3441,16 +3605,16 @@
         <v>27</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -3657,7 +3821,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>41</v>
@@ -3695,10 +3859,10 @@
         <v>12000</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>35</v>
@@ -3721,10 +3885,10 @@
         <v>13000</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>38</v>
@@ -3747,10 +3911,10 @@
         <v>15000</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>38</v>
@@ -3773,10 +3937,10 @@
         <v>15001</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>38</v>
@@ -3799,10 +3963,10 @@
         <v>15002</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>38</v>
@@ -3825,10 +3989,10 @@
         <v>15003</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>38</v>
@@ -3851,10 +4015,10 @@
         <v>15004</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>38</v>
@@ -3877,10 +4041,10 @@
         <v>15005</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>38</v>
@@ -3903,10 +4067,10 @@
         <v>15006</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>38</v>
@@ -3929,10 +4093,10 @@
         <v>15007</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>38</v>
@@ -3955,10 +4119,10 @@
         <v>15008</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>38</v>
@@ -3981,10 +4145,10 @@
         <v>15009</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>38</v>
@@ -4007,10 +4171,10 @@
         <v>15010</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>38</v>
@@ -4033,10 +4197,10 @@
         <v>15011</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>38</v>
@@ -4059,10 +4223,10 @@
         <v>15012</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>38</v>
@@ -4085,10 +4249,10 @@
         <v>15013</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C22" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>38</v>
@@ -4111,10 +4275,10 @@
         <v>15014</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C23" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>38</v>
@@ -4137,10 +4301,10 @@
         <v>15015</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C24" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>38</v>
@@ -4163,10 +4327,10 @@
         <v>15016</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C25" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>38</v>
@@ -4189,10 +4353,10 @@
         <v>15017</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>38</v>
@@ -4215,10 +4379,10 @@
         <v>15018</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C27" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>38</v>
@@ -4243,39 +4407,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="10.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="9.1796875" style="9"/>
+    <col min="2" max="2" width="10.7265625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="53.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5">
+    <row r="1" spans="1:5" ht="17">
       <c r="A1" s="10" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4286,7 +4450,7 @@
         <v>15000</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D2" s="9">
         <v>0</v>
@@ -4303,7 +4467,7 @@
         <v>15001</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D3" s="9">
         <v>0</v>
@@ -4320,7 +4484,7 @@
         <v>15002</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D4" s="9">
         <v>0</v>
@@ -4337,7 +4501,7 @@
         <v>15003</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D5" s="9">
         <v>0</v>
@@ -4354,7 +4518,7 @@
         <v>15004</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D6" s="9">
         <v>0</v>
@@ -4371,7 +4535,7 @@
         <v>15005</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D7" s="9">
         <v>0</v>
@@ -4388,7 +4552,7 @@
         <v>15006</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D8" s="9">
         <v>0</v>
@@ -4405,7 +4569,7 @@
         <v>15007</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D9" s="9">
         <v>0</v>
@@ -4422,7 +4586,7 @@
         <v>15008</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D10" s="9">
         <v>0</v>
@@ -4439,7 +4603,7 @@
         <v>15009</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D11" s="9">
         <v>0</v>
@@ -4456,7 +4620,7 @@
         <v>15010</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D12" s="9">
         <v>0</v>
@@ -4473,7 +4637,7 @@
         <v>15011</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D13" s="9">
         <v>0</v>
@@ -4490,7 +4654,7 @@
         <v>15012</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -4507,7 +4671,7 @@
         <v>15013</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D15" s="9">
         <v>0</v>
@@ -4524,7 +4688,7 @@
         <v>15014</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D16" s="9">
         <v>0</v>
@@ -4541,7 +4705,7 @@
         <v>15015</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D17" s="9">
         <v>3</v>
@@ -4558,7 +4722,7 @@
         <v>15016</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D18" s="9">
         <v>0</v>
@@ -4575,7 +4739,7 @@
         <v>15017</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D19" s="9">
         <v>0</v>
@@ -4592,7 +4756,7 @@
         <v>15018</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D20" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'main' into InventoryUI_RWJ""
This reverts commit 638c69102483d8c75a1c9c39d9044904ff3cf151.
</commit_message>
<xml_diff>
--- a/KGA_SUPERmetaVR/Assets/Sheet/Data.xlsx
+++ b/KGA_SUPERmetaVR/Assets/Sheet/Data.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohgo\Desktop\Unity\SUPERmetaVR\KGA_SUPERmetaVR\KGA_SUPERmetaVR\Assets\Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Slime\VR\SUPERmeta\KGA_SUPERmetaVR\Assets\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA00017-3EEA-4F4C-89EB-4FFE03E432B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NoticePopup" sheetId="1" r:id="rId1"/>
-    <sheet name="NPCDialogue" sheetId="5" r:id="rId2"/>
-    <sheet name="PeekabooCustomizing" sheetId="2" r:id="rId3"/>
-    <sheet name="SpeechBubbleSheet" sheetId="3" r:id="rId4"/>
-    <sheet name="ItemSheet" sheetId="4" r:id="rId5"/>
-    <sheet name="RewardSheet" sheetId="6" r:id="rId6"/>
+    <sheet name="NPCSheet" sheetId="7" r:id="rId2"/>
+    <sheet name="NPCDialogue" sheetId="5" r:id="rId3"/>
+    <sheet name="PeekabooCustomizing" sheetId="2" r:id="rId4"/>
+    <sheet name="SpeechBubbleSheet" sheetId="3" r:id="rId5"/>
+    <sheet name="ItemSheet" sheetId="4" r:id="rId6"/>
+    <sheet name="RewardSheet" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="216">
   <si>
     <t>id</t>
   </si>
@@ -585,9 +585,6 @@
 네 잎 클로버를 4개 모으면 말해!</t>
   </si>
   <si>
-    <t>코스튬이 갖고 싶으면 네 잎 클로버 4개를 가져와!</t>
-  </si>
-  <si>
     <t>안녕, 친구.
 재미있는 놀이가 하나 있는데 이야기해줄까?</t>
   </si>
@@ -816,564 +813,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>개를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>모았으면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>언제든지</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>말을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>걸어</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>!</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>안녕</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>나는</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>코티야</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>네</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>잎</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>클로버를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>개</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>가져오면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>코스튬으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>변화시켜줄게</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>됐어</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-! </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>이쁘게</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>착용해</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-!</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>좋아</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ~
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>우리</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>미니마니모</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>마을엔</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>인간과</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>사이좋게</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>지내고싶은</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>도깨비들이</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>많아</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>네잎클로버</t>
   </si>
   <si>
@@ -1547,11 +986,165 @@
     <t>Sword</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>SoudEffect</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetItemID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetItemEA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OutItemID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OutItemEA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TT_Mo_1.wav</t>
+  </si>
+  <si>
+    <t>TT_Mo_2.wav</t>
+  </si>
+  <si>
+    <t>TT_Mo_3.wav</t>
+  </si>
+  <si>
+    <t>TT_Cu_1.wav</t>
+  </si>
+  <si>
+    <t>TT_Cu_3.mp3</t>
+  </si>
+  <si>
+    <t>TT_Cu_2.mp3</t>
+  </si>
+  <si>
+    <t>안녕? 적응은 잘 하고있어? 즐거운 하루 보내!</t>
+  </si>
+  <si>
+    <t>나는 여기서 항상 새로운 어린이들을 인도해!</t>
+  </si>
+  <si>
+    <t>쿠가 좀 까칠하지? 하지만 마음은 따듯한 녀석이야-</t>
+  </si>
+  <si>
+    <t>이 쿠님이 보고싶어서 왔나?</t>
+  </si>
+  <si>
+    <t>어린이- 저기가서 놀아- 이 쿠님은 바쁘다고-</t>
+  </si>
+  <si>
+    <t>안녕- 나는 코티야. 네 잎 클로버를 4개 가져오면 코스튬으로 변화시켜줄게</t>
+  </si>
+  <si>
+    <t>CC_Coty_1.mp3</t>
+  </si>
+  <si>
+    <t>4개를 모았으면 언제든지 말을 걸어!</t>
+  </si>
+  <si>
+    <t>CC_Coty_2.mp3</t>
+  </si>
+  <si>
+    <t>CC_Coty_3.mp3</t>
+  </si>
+  <si>
+    <t>다 됐어-! 이쁘게 착용해-!</t>
+  </si>
+  <si>
+    <t>CC_Coty_4.mp3</t>
+  </si>
+  <si>
+    <t>음? 코스튬이 갖고 싶으면 네 잎 클로버 4개를 가져와!</t>
+  </si>
+  <si>
+    <t>CC_Coty_5.mp3</t>
+  </si>
+  <si>
+    <t>PK_BOO_1.mp3</t>
+  </si>
+  <si>
+    <t>좋아 ~
+우리 미니마니모 마을엔 인간과 사이좋게 지내고싶은 도깨비들이 많아</t>
+  </si>
+  <si>
+    <t>PK_BOO_2.mp3</t>
+  </si>
+  <si>
+    <t>모</t>
+  </si>
+  <si>
+    <t>쿠</t>
+  </si>
+  <si>
+    <t>코티</t>
+  </si>
+  <si>
+    <t>부</t>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ame</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ype</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nimation</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
@@ -1921,23 +1514,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" style="9" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="9" customWidth="1"/>
     <col min="3" max="3" width="92" style="9" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="9" customWidth="1"/>
     <col min="6" max="7" width="9" style="9" customWidth="1"/>
-    <col min="8" max="27" width="8.7265625" style="9" customWidth="1"/>
-    <col min="28" max="16384" width="14.453125" style="9"/>
+    <col min="8" max="27" width="8.7109375" style="9" customWidth="1"/>
+    <col min="28" max="16384" width="14.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.5" customHeight="1">
@@ -1979,7 +1572,7 @@
       <c r="Z1" s="6"/>
       <c r="AA1" s="6"/>
     </row>
-    <row r="2" spans="1:27" ht="29">
+    <row r="2" spans="1:27" ht="30">
       <c r="A2" s="11">
         <v>0</v>
       </c>
@@ -2244,7 +1837,7 @@
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
     </row>
-    <row r="9" spans="1:27" ht="29">
+    <row r="9" spans="1:27" ht="30">
       <c r="A9" s="11">
         <v>52004</v>
       </c>
@@ -2429,7 +2022,7 @@
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
     </row>
-    <row r="14" spans="1:27" ht="29">
+    <row r="14" spans="1:27" ht="30">
       <c r="A14" s="11">
         <v>52009</v>
       </c>
@@ -2489,71 +2082,168 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="9.1796875" style="15"/>
-    <col min="4" max="4" width="82.54296875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="15" customWidth="1"/>
-    <col min="6" max="9" width="29.26953125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" style="15" customWidth="1"/>
-    <col min="11" max="14" width="29.26953125" style="15" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="16"/>
+    <col min="1" max="3" width="9.140625" style="9"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="15" customFormat="1">
+    <row r="1" spans="1:4" s="9" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="9">
+        <v>20000</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="9">
+        <v>20001</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="9">
+        <v>20300</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="9">
+        <v>20600</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="15"/>
+    <col min="4" max="4" width="82.5703125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="15" customWidth="1"/>
+    <col min="6" max="9" width="29.28515625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="15" customWidth="1"/>
+    <col min="11" max="14" width="29.28515625" style="15" customWidth="1"/>
+    <col min="15" max="20" width="14.85546875" style="16" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="15" customFormat="1">
       <c r="A1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="N1" s="11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="15">
-        <v>21001</v>
+        <v>21000</v>
       </c>
       <c r="B2" s="15">
         <v>20000</v>
@@ -2562,10 +2252,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="29">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="30">
       <c r="A3" s="15">
         <v>21001</v>
       </c>
@@ -2573,13 +2263,16 @@
         <v>20000</v>
       </c>
       <c r="C3" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="29">
+      <c r="O3" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="30">
       <c r="A4" s="15">
         <v>21001</v>
       </c>
@@ -2587,13 +2280,16 @@
         <v>20000</v>
       </c>
       <c r="C4" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="29">
+      <c r="O4" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="30">
       <c r="A5" s="15">
         <v>21001</v>
       </c>
@@ -2601,13 +2297,13 @@
         <v>20000</v>
       </c>
       <c r="C5" s="15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="29">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="30">
       <c r="A6" s="15">
         <v>21001</v>
       </c>
@@ -2615,13 +2311,13 @@
         <v>20000</v>
       </c>
       <c r="C6" s="15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:20">
       <c r="A7" s="15">
         <v>21001</v>
       </c>
@@ -2629,13 +2325,13 @@
         <v>20000</v>
       </c>
       <c r="C7" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="29">
+    <row r="8" spans="1:20" ht="30">
       <c r="A8" s="15">
         <v>21001</v>
       </c>
@@ -2643,13 +2339,16 @@
         <v>20000</v>
       </c>
       <c r="C8" s="15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="20" customFormat="1" ht="29">
+        <v>109</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="20" customFormat="1" ht="30">
       <c r="A9" s="18">
         <v>21002</v>
       </c>
@@ -2673,7 +2372,7 @@
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
     </row>
-    <row r="10" spans="1:14" ht="29">
+    <row r="10" spans="1:20" ht="30">
       <c r="A10" s="15">
         <v>21003</v>
       </c>
@@ -2684,10 +2383,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>110</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="15">
         <v>21003</v>
       </c>
@@ -2701,7 +2403,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="20" customFormat="1">
+    <row r="12" spans="1:20" s="20" customFormat="1">
       <c r="A12" s="18">
         <v>21004</v>
       </c>
@@ -2712,7 +2414,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -2724,8 +2426,11 @@
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
-    </row>
-    <row r="13" spans="1:14" s="20" customFormat="1" ht="29">
+      <c r="O12" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="20" customFormat="1" ht="30">
       <c r="A13" s="18">
         <v>21004</v>
       </c>
@@ -2736,7 +2441,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
@@ -2749,7 +2454,7 @@
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="1:14" ht="29">
+    <row r="14" spans="1:20" ht="30">
       <c r="A14" s="15">
         <v>21005</v>
       </c>
@@ -2763,7 +2468,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="29">
+    <row r="15" spans="1:20" ht="30">
       <c r="A15" s="15">
         <v>21005</v>
       </c>
@@ -2777,7 +2482,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="29">
+    <row r="16" spans="1:20" ht="30">
       <c r="A16" s="15">
         <v>21005</v>
       </c>
@@ -2791,7 +2496,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="29">
+    <row r="17" spans="1:19" ht="30">
       <c r="A17" s="15">
         <v>21005</v>
       </c>
@@ -2802,10 +2507,13 @@
         <v>4</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="29">
+        <v>113</v>
+      </c>
+      <c r="O17" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="30">
       <c r="A18" s="15">
         <v>21005</v>
       </c>
@@ -2816,10 +2524,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="15">
         <v>21005</v>
       </c>
@@ -2830,21 +2538,21 @@
         <v>6</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" s="20" customFormat="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" s="20" customFormat="1">
       <c r="A20" s="18">
-        <v>24000</v>
+        <v>21006</v>
       </c>
       <c r="B20" s="18">
-        <v>20300</v>
+        <v>20000</v>
       </c>
       <c r="C20" s="18">
         <v>1</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>131</v>
+        <v>192</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
@@ -2856,19 +2564,22 @@
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-    </row>
-    <row r="21" spans="1:14" s="20" customFormat="1">
+      <c r="O20" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" s="20" customFormat="1">
       <c r="A21" s="18">
-        <v>24000</v>
+        <v>21007</v>
       </c>
       <c r="B21" s="18">
-        <v>20300</v>
+        <v>20000</v>
       </c>
       <c r="C21" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
@@ -2880,48 +2591,39 @@
       <c r="L21" s="18"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="O21" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="15">
-        <v>24001</v>
+        <v>21008</v>
       </c>
       <c r="B22" s="15">
-        <v>20300</v>
+        <v>20000</v>
       </c>
       <c r="C22" s="15">
         <v>1</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="H22" s="15">
-        <v>24002</v>
-      </c>
-      <c r="I22" s="15">
-        <v>24003</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="N22" s="15">
-        <v>24004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="20" customFormat="1">
+        <v>194</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" s="20" customFormat="1">
       <c r="A23" s="18">
-        <v>24002</v>
+        <v>21009</v>
       </c>
       <c r="B23" s="18">
-        <v>20300</v>
+        <v>20001</v>
       </c>
       <c r="C23" s="18">
         <v>1</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>84</v>
+        <v>195</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
@@ -2934,18 +2636,18 @@
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="1:14" s="20" customFormat="1">
+    <row r="24" spans="1:19" s="20" customFormat="1">
       <c r="A24" s="18">
-        <v>24002</v>
+        <v>21010</v>
       </c>
       <c r="B24" s="18">
-        <v>20300</v>
+        <v>20001</v>
       </c>
       <c r="C24" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>132</v>
+        <v>196</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
@@ -2958,9 +2660,9 @@
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="1:14" ht="29">
+    <row r="25" spans="1:19">
       <c r="A25" s="15">
-        <v>24003</v>
+        <v>24000</v>
       </c>
       <c r="B25" s="15">
         <v>20300</v>
@@ -2969,21 +2671,24 @@
         <v>1</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="20" customFormat="1">
+        <v>197</v>
+      </c>
+      <c r="O25" s="16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" s="20" customFormat="1">
       <c r="A26" s="18">
-        <v>24004</v>
+        <v>24000</v>
       </c>
       <c r="B26" s="18">
         <v>20300</v>
       </c>
       <c r="C26" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>86</v>
+        <v>199</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
@@ -2996,44 +2701,56 @@
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
     </row>
-    <row r="27" spans="1:14" ht="29">
+    <row r="27" spans="1:19">
       <c r="A27" s="15">
-        <v>27000</v>
+        <v>24001</v>
       </c>
       <c r="B27" s="15">
-        <v>20600</v>
+        <v>20300</v>
       </c>
       <c r="C27" s="15">
         <v>1</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>88</v>
+        <v>82</v>
+      </c>
+      <c r="F27" s="15">
+        <v>12000</v>
+      </c>
+      <c r="G27" s="15">
+        <v>4</v>
+      </c>
+      <c r="H27" s="15">
+        <v>24002</v>
       </c>
       <c r="I27" s="15">
-        <v>27002</v>
+        <v>24003</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="N27" s="15">
-        <v>27001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="20" customFormat="1" ht="29">
+        <v>24004</v>
+      </c>
+      <c r="O27" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" s="20" customFormat="1">
       <c r="A28" s="18">
-        <v>27001</v>
+        <v>24002</v>
       </c>
       <c r="B28" s="18">
-        <v>20600</v>
+        <v>20300</v>
       </c>
       <c r="C28" s="18">
         <v>1</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
@@ -3045,92 +2762,116 @@
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
-    </row>
-    <row r="29" spans="1:14" ht="29">
+      <c r="O28" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="15">
-        <v>27002</v>
+        <v>24002</v>
       </c>
       <c r="B29" s="15">
-        <v>20600</v>
+        <v>20300</v>
       </c>
       <c r="C29" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="29">
+        <v>202</v>
+      </c>
+      <c r="P29" s="16">
+        <v>13000</v>
+      </c>
+      <c r="Q29" s="16">
+        <v>1</v>
+      </c>
+      <c r="R29" s="16">
+        <v>12000</v>
+      </c>
+      <c r="S29" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="30">
       <c r="A30" s="15">
-        <v>27002</v>
+        <v>24003</v>
       </c>
       <c r="B30" s="15">
-        <v>20600</v>
+        <v>20300</v>
       </c>
       <c r="C30" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="29">
+        <v>85</v>
+      </c>
+      <c r="O30" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="15">
-        <v>27002</v>
+        <v>24004</v>
       </c>
       <c r="B31" s="15">
-        <v>20600</v>
+        <v>20300</v>
       </c>
       <c r="C31" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+        <v>204</v>
+      </c>
+      <c r="O31" s="16" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="30">
       <c r="A32" s="15">
-        <v>27002</v>
+        <v>27000</v>
       </c>
       <c r="B32" s="15">
         <v>20600</v>
       </c>
       <c r="C32" s="15">
-        <v>4</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="29">
+        <v>1</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I32" s="15">
+        <v>27002</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="N32" s="15">
+        <v>27001</v>
+      </c>
+      <c r="O32" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="30">
       <c r="A33" s="15">
-        <v>27002</v>
+        <v>27001</v>
       </c>
       <c r="B33" s="15">
         <v>20600</v>
       </c>
       <c r="C33" s="15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="I33" s="15">
-        <v>27006</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="N33" s="15">
-        <v>27003</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" s="20" customFormat="1" ht="29">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="20" customFormat="1" ht="30">
       <c r="A34" s="18">
-        <v>27003</v>
+        <v>27002</v>
       </c>
       <c r="B34" s="18">
         <v>20600</v>
@@ -3139,136 +2880,231 @@
         <v>1</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>98</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
-      <c r="I34" s="18">
-        <v>27004</v>
-      </c>
-      <c r="J34" s="18" t="s">
-        <v>99</v>
-      </c>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
-      <c r="N34" s="18">
-        <v>27001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="29">
+      <c r="N34" s="18"/>
+    </row>
+    <row r="35" spans="1:15" ht="30">
       <c r="A35" s="15">
-        <v>27004</v>
+        <v>27002</v>
       </c>
       <c r="B35" s="15">
         <v>20600</v>
       </c>
       <c r="C35" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" s="20" customFormat="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="20" customFormat="1" ht="30">
       <c r="A36" s="18">
-        <v>27005</v>
+        <v>27002</v>
       </c>
       <c r="B36" s="18">
         <v>20600</v>
       </c>
       <c r="C36" s="18">
-        <v>1</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>98</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
-      <c r="I36" s="18">
-        <v>27004</v>
-      </c>
-      <c r="J36" s="18" t="s">
-        <v>99</v>
-      </c>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
       <c r="K36" s="18"/>
       <c r="L36" s="18"/>
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:15">
       <c r="A37" s="15">
-        <v>27006</v>
+        <v>27002</v>
       </c>
       <c r="B37" s="15">
         <v>20600</v>
       </c>
       <c r="C37" s="15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="29">
+        <v>92</v>
+      </c>
+      <c r="O37" s="16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="30">
       <c r="A38" s="15">
-        <v>27006</v>
+        <v>27002</v>
       </c>
       <c r="B38" s="15">
         <v>20600</v>
       </c>
       <c r="C38" s="15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+        <v>93</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="15">
+        <v>27006</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="N38" s="15">
+        <v>27003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="30">
       <c r="A39" s="15">
-        <v>27006</v>
+        <v>27003</v>
       </c>
       <c r="B39" s="15">
         <v>20600</v>
       </c>
       <c r="C39" s="15">
-        <v>3</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>1</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I39" s="15">
+        <v>27004</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="N39" s="15">
+        <v>27001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="30">
       <c r="A40" s="15">
-        <v>27006</v>
+        <v>27004</v>
       </c>
       <c r="B40" s="15">
         <v>20600</v>
       </c>
       <c r="C40" s="15">
+        <v>1</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="15">
+        <v>27005</v>
+      </c>
+      <c r="B41" s="15">
+        <v>20600</v>
+      </c>
+      <c r="C41" s="15">
+        <v>1</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I41" s="15">
+        <v>27004</v>
+      </c>
+      <c r="J41" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O41" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="15">
+        <v>27006</v>
+      </c>
+      <c r="B42" s="15">
+        <v>20600</v>
+      </c>
+      <c r="C42" s="15">
+        <v>1</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="30">
+      <c r="A43" s="15">
+        <v>27006</v>
+      </c>
+      <c r="B43" s="15">
+        <v>20600</v>
+      </c>
+      <c r="C43" s="15">
+        <v>2</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="15">
+        <v>27006</v>
+      </c>
+      <c r="B44" s="15">
+        <v>20600</v>
+      </c>
+      <c r="C44" s="15">
+        <v>3</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="15">
+        <v>27006</v>
+      </c>
+      <c r="B45" s="15">
+        <v>20600</v>
+      </c>
+      <c r="C45" s="15">
         <v>4</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D45" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="I45" s="15">
+        <v>27003</v>
+      </c>
+      <c r="J45" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="I40" s="15">
-        <v>27003</v>
-      </c>
-      <c r="J40" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="N40" s="15">
+      <c r="N45" s="15">
         <v>27006</v>
       </c>
     </row>
@@ -3279,20 +3115,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="4" width="28.26953125" customWidth="1"/>
-    <col min="5" max="26" width="8.7265625" customWidth="1"/>
+    <col min="1" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" customHeight="1">
@@ -3386,20 +3222,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="66.81640625" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" customWidth="1"/>
     <col min="3" max="6" width="9" customWidth="1"/>
-    <col min="7" max="26" width="8.7265625" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1">
@@ -3569,23 +3405,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="78.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="13" style="9" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="26" width="8.7265625" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="9" customFormat="1" ht="16.5" customHeight="1">
@@ -3605,16 +3441,16 @@
         <v>27</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -3821,7 +3657,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>41</v>
@@ -3859,10 +3695,10 @@
         <v>12000</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>35</v>
@@ -3885,10 +3721,10 @@
         <v>13000</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>38</v>
@@ -3911,10 +3747,10 @@
         <v>15000</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>38</v>
@@ -3937,10 +3773,10 @@
         <v>15001</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>38</v>
@@ -3963,10 +3799,10 @@
         <v>15002</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>38</v>
@@ -3989,10 +3825,10 @@
         <v>15003</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>38</v>
@@ -4015,10 +3851,10 @@
         <v>15004</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>38</v>
@@ -4041,10 +3877,10 @@
         <v>15005</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>38</v>
@@ -4067,10 +3903,10 @@
         <v>15006</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>38</v>
@@ -4093,10 +3929,10 @@
         <v>15007</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>38</v>
@@ -4119,10 +3955,10 @@
         <v>15008</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>38</v>
@@ -4145,10 +3981,10 @@
         <v>15009</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>38</v>
@@ -4171,10 +4007,10 @@
         <v>15010</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>38</v>
@@ -4197,10 +4033,10 @@
         <v>15011</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>38</v>
@@ -4223,10 +4059,10 @@
         <v>15012</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C21" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>38</v>
@@ -4249,10 +4085,10 @@
         <v>15013</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>38</v>
@@ -4275,10 +4111,10 @@
         <v>15014</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>38</v>
@@ -4301,10 +4137,10 @@
         <v>15015</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C24" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>38</v>
@@ -4327,10 +4163,10 @@
         <v>15016</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C25" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>38</v>
@@ -4353,10 +4189,10 @@
         <v>15017</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C26" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>38</v>
@@ -4379,10 +4215,10 @@
         <v>15018</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C27" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>38</v>
@@ -4407,39 +4243,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="9"/>
-    <col min="2" max="2" width="10.7265625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="53.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="9"/>
+    <col min="1" max="1" width="9.140625" style="9"/>
+    <col min="2" max="2" width="10.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17">
+    <row r="1" spans="1:5" ht="16.5">
       <c r="A1" s="10" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4450,7 +4286,7 @@
         <v>15000</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D2" s="9">
         <v>0</v>
@@ -4467,7 +4303,7 @@
         <v>15001</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D3" s="9">
         <v>0</v>
@@ -4484,7 +4320,7 @@
         <v>15002</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D4" s="9">
         <v>0</v>
@@ -4501,7 +4337,7 @@
         <v>15003</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D5" s="9">
         <v>0</v>
@@ -4518,7 +4354,7 @@
         <v>15004</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D6" s="9">
         <v>0</v>
@@ -4535,7 +4371,7 @@
         <v>15005</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D7" s="9">
         <v>0</v>
@@ -4552,7 +4388,7 @@
         <v>15006</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D8" s="9">
         <v>0</v>
@@ -4569,7 +4405,7 @@
         <v>15007</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D9" s="9">
         <v>0</v>
@@ -4586,7 +4422,7 @@
         <v>15008</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D10" s="9">
         <v>0</v>
@@ -4603,7 +4439,7 @@
         <v>15009</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D11" s="9">
         <v>0</v>
@@ -4620,7 +4456,7 @@
         <v>15010</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D12" s="9">
         <v>0</v>
@@ -4637,7 +4473,7 @@
         <v>15011</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D13" s="9">
         <v>0</v>
@@ -4654,7 +4490,7 @@
         <v>15012</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -4671,7 +4507,7 @@
         <v>15013</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D15" s="9">
         <v>0</v>
@@ -4688,7 +4524,7 @@
         <v>15014</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D16" s="9">
         <v>0</v>
@@ -4705,7 +4541,7 @@
         <v>15015</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D17" s="9">
         <v>3</v>
@@ -4722,7 +4558,7 @@
         <v>15016</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D18" s="9">
         <v>0</v>
@@ -4739,7 +4575,7 @@
         <v>15017</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D19" s="9">
         <v>0</v>
@@ -4756,7 +4592,7 @@
         <v>15018</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D20" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' into SecondQAInventory_RWJ"
This reverts commit 93c4a5fb09d8e80348e010bff4f48699379e51f1, reversing
changes made to f97ccbc4c17f645016cd689db338d9486e627f66.
</commit_message>
<xml_diff>
--- a/KGA_SUPERmetaVR/Assets/Sheet/Data.xlsx
+++ b/KGA_SUPERmetaVR/Assets/Sheet/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Slime\VR\SUPERmeta\KGA_SUPERmetaVR\Assets\Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohgo\Desktop\Unity\SUPERmetaVR\KGA_SUPERmetaVR\KGA_SUPERmetaVR\Assets\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C862C13-77C8-4277-AA6B-A4E6370A648B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NoticePopup" sheetId="1" r:id="rId1"/>
@@ -1147,7 +1148,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
@@ -1226,7 +1227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1302,9 +1303,6 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1520,23 +1518,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" style="9" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" style="9" customWidth="1"/>
     <col min="3" max="3" width="92" style="9" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" style="9" customWidth="1"/>
     <col min="6" max="7" width="9" style="9" customWidth="1"/>
-    <col min="8" max="27" width="8.7109375" style="9" customWidth="1"/>
-    <col min="28" max="16384" width="14.42578125" style="9"/>
+    <col min="8" max="27" width="8.7265625" style="9" customWidth="1"/>
+    <col min="28" max="16384" width="14.453125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.5" customHeight="1">
@@ -1578,7 +1576,7 @@
       <c r="Z1" s="6"/>
       <c r="AA1" s="6"/>
     </row>
-    <row r="2" spans="1:27" ht="30">
+    <row r="2" spans="1:27" ht="29">
       <c r="A2" s="11">
         <v>0</v>
       </c>
@@ -1843,7 +1841,7 @@
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
     </row>
-    <row r="9" spans="1:27" ht="30">
+    <row r="9" spans="1:27" ht="29">
       <c r="A9" s="11">
         <v>52004</v>
       </c>
@@ -2028,7 +2026,7 @@
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
     </row>
-    <row r="14" spans="1:27" ht="30">
+    <row r="14" spans="1:27" ht="29">
       <c r="A14" s="11">
         <v>52009</v>
       </c>
@@ -2088,17 +2086,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="9"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="1" max="3" width="9.1796875" style="9"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1">
@@ -2166,23 +2164,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="15"/>
-    <col min="4" max="4" width="82.5703125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="15" customWidth="1"/>
-    <col min="6" max="9" width="29.28515625" style="15" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="15" customWidth="1"/>
-    <col min="11" max="14" width="29.28515625" style="15" customWidth="1"/>
-    <col min="15" max="20" width="14.85546875" style="16" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="3" width="9.1796875" style="15"/>
+    <col min="4" max="4" width="82.54296875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="15" customWidth="1"/>
+    <col min="6" max="9" width="29.26953125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" style="15" customWidth="1"/>
+    <col min="11" max="14" width="29.26953125" style="15" customWidth="1"/>
+    <col min="15" max="20" width="14.81640625" style="16" customWidth="1"/>
+    <col min="21" max="16384" width="9.1796875" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="15" customFormat="1">
@@ -2261,7 +2259,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="30">
+    <row r="3" spans="1:20" ht="29">
       <c r="A3" s="15">
         <v>21001</v>
       </c>
@@ -2278,7 +2276,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="30">
+    <row r="4" spans="1:20" ht="29">
       <c r="A4" s="15">
         <v>21001</v>
       </c>
@@ -2295,7 +2293,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="30">
+    <row r="5" spans="1:20" ht="29">
       <c r="A5" s="15">
         <v>21001</v>
       </c>
@@ -2309,7 +2307,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="30">
+    <row r="6" spans="1:20" ht="29">
       <c r="A6" s="15">
         <v>21001</v>
       </c>
@@ -2337,7 +2335,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="30">
+    <row r="8" spans="1:20" ht="29">
       <c r="A8" s="15">
         <v>21001</v>
       </c>
@@ -2354,7 +2352,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="20" customFormat="1" ht="30">
+    <row r="9" spans="1:20" s="20" customFormat="1" ht="29">
       <c r="A9" s="18">
         <v>21002</v>
       </c>
@@ -2378,7 +2376,7 @@
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
     </row>
-    <row r="10" spans="1:20" ht="30">
+    <row r="10" spans="1:20" ht="29">
       <c r="A10" s="15">
         <v>21003</v>
       </c>
@@ -2436,7 +2434,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="20" customFormat="1" ht="30">
+    <row r="13" spans="1:20" s="20" customFormat="1" ht="29">
       <c r="A13" s="18">
         <v>21004</v>
       </c>
@@ -2460,7 +2458,7 @@
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="1:20" ht="30">
+    <row r="14" spans="1:20" ht="29">
       <c r="A14" s="15">
         <v>21005</v>
       </c>
@@ -2474,7 +2472,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="30">
+    <row r="15" spans="1:20" ht="29">
       <c r="A15" s="15">
         <v>21005</v>
       </c>
@@ -2488,7 +2486,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="30">
+    <row r="16" spans="1:20" ht="29">
       <c r="A16" s="15">
         <v>21005</v>
       </c>
@@ -2502,7 +2500,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="30">
+    <row r="17" spans="1:19" ht="29">
       <c r="A17" s="15">
         <v>21005</v>
       </c>
@@ -2519,7 +2517,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="30">
+    <row r="18" spans="1:19" ht="29">
       <c r="A18" s="15">
         <v>21005</v>
       </c>
@@ -2696,7 +2694,7 @@
       <c r="D26" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="E26" s="26"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
@@ -2798,7 +2796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="30">
+    <row r="30" spans="1:19" ht="29">
       <c r="A30" s="15">
         <v>24003</v>
       </c>
@@ -2832,7 +2830,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="30">
+    <row r="32" spans="1:19" ht="29">
       <c r="A32" s="15">
         <v>27000</v>
       </c>
@@ -2861,7 +2859,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="30">
+    <row r="33" spans="1:15" ht="29">
       <c r="A33" s="15">
         <v>27001</v>
       </c>
@@ -2875,7 +2873,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="20" customFormat="1" ht="30">
+    <row r="34" spans="1:15" s="20" customFormat="1" ht="29">
       <c r="A34" s="18">
         <v>27002</v>
       </c>
@@ -2899,7 +2897,7 @@
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="1:15" ht="30">
+    <row r="35" spans="1:15" ht="29">
       <c r="A35" s="15">
         <v>27002</v>
       </c>
@@ -2913,7 +2911,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="20" customFormat="1" ht="30">
+    <row r="36" spans="1:15" s="20" customFormat="1" ht="29">
       <c r="A36" s="18">
         <v>27002</v>
       </c>
@@ -2954,7 +2952,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="30">
+    <row r="38" spans="1:15" ht="29">
       <c r="A38" s="15">
         <v>27002</v>
       </c>
@@ -2980,7 +2978,7 @@
         <v>27003</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="30">
+    <row r="39" spans="1:15" ht="29">
       <c r="A39" s="15">
         <v>27003</v>
       </c>
@@ -3006,7 +3004,7 @@
         <v>27001</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="30">
+    <row r="40" spans="1:15" ht="29">
       <c r="A40" s="15">
         <v>27004</v>
       </c>
@@ -3060,7 +3058,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="30">
+    <row r="43" spans="1:15" ht="29">
       <c r="A43" s="15">
         <v>27006</v>
       </c>
@@ -3122,19 +3120,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
-    <col min="5" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="2" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="4" width="28.26953125" customWidth="1"/>
+    <col min="5" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" customHeight="1">
@@ -3229,19 +3227,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="66.85546875" customWidth="1"/>
+    <col min="2" max="2" width="66.81640625" customWidth="1"/>
     <col min="3" max="6" width="9" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="7" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1">
@@ -3412,22 +3410,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="78.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
     <col min="5" max="5" width="13" style="9" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="7" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="9" customFormat="1" ht="16.5" customHeight="1">
@@ -4250,24 +4248,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="10.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="9.1796875" style="9"/>
+    <col min="2" max="2" width="10.7265625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="53.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5">
+    <row r="1" spans="1:5" ht="17">
       <c r="A1" s="10" t="s">
         <v>177</v>
       </c>

</xml_diff>